<commit_message>
updating BOM with tank mount parts
</commit_message>
<xml_diff>
--- a/hardware-distribution/bill-of-materials.xlsx
+++ b/hardware-distribution/bill-of-materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morgan\Documents\PhD Git Repos\open-UST\hardware-distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C024DF-70AD-443B-88AA-F7D2E23042B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095F0CA8-D741-4C72-AA3B-F56CF5BC8204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="3660" windowWidth="14430" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="198">
   <si>
     <t>Off the shelf items</t>
   </si>
@@ -554,6 +554,69 @@
   </si>
   <si>
     <t>Part ID</t>
+  </si>
+  <si>
+    <t>M3 x 30mm Hex Socket Cap Screw Black</t>
+  </si>
+  <si>
+    <t>467-9846</t>
+  </si>
+  <si>
+    <t>RS 467-9846</t>
+  </si>
+  <si>
+    <t>M3 x 8mm Hex Socket Button Screw</t>
+  </si>
+  <si>
+    <t>281-186</t>
+  </si>
+  <si>
+    <t>RS 281-186</t>
+  </si>
+  <si>
+    <t>(for plug)</t>
+  </si>
+  <si>
+    <t>M3 x 6mm Hex Socket Button Screw</t>
+  </si>
+  <si>
+    <t>822-9098</t>
+  </si>
+  <si>
+    <t>RS 822-9098</t>
+  </si>
+  <si>
+    <t>M3 x 10mm Hex Socket Button Screw</t>
+  </si>
+  <si>
+    <t>281-192</t>
+  </si>
+  <si>
+    <t>RS 281-192</t>
+  </si>
+  <si>
+    <t>850-8476</t>
+  </si>
+  <si>
+    <t>RS 850-8476</t>
+  </si>
+  <si>
+    <t>RS PRO Silver Aluminium Strut, 20 x 20 mm, 5mm Groove , 1000mm Length</t>
+  </si>
+  <si>
+    <t>RS PRO Connecting Component, T-Slot Nut, strut profile 20 mm, groove Size 5mm</t>
+  </si>
+  <si>
+    <t>180-9109</t>
+  </si>
+  <si>
+    <t>RS 180-9109</t>
+  </si>
+  <si>
+    <t>Tank Mount</t>
+  </si>
+  <si>
+    <t>M6 x 16 mmm stainless steel screws</t>
   </si>
 </sst>
 </file>
@@ -563,7 +626,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-m"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -574,6 +637,7 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -581,6 +645,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -588,6 +653,7 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -595,12 +661,14 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -608,6 +676,7 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -616,6 +685,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -623,20 +693,38 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +737,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -659,10 +753,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -713,8 +808,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -931,10 +1040,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1027"/>
+  <dimension ref="A1:H1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -948,7 +1057,7 @@
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -956,7 +1065,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -966,7 +1075,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -974,7 +1083,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>176</v>
       </c>
@@ -997,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>131</v>
       </c>
@@ -1020,7 +1129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>132</v>
       </c>
@@ -1043,7 +1152,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>133</v>
       </c>
@@ -1066,7 +1175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>134</v>
       </c>
@@ -1089,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>135</v>
       </c>
@@ -1112,7 +1221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>136</v>
       </c>
@@ -1135,7 +1244,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>137</v>
       </c>
@@ -1158,7 +1267,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>138</v>
       </c>
@@ -1181,7 +1290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>139</v>
       </c>
@@ -1204,589 +1313,599 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="5">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="8">
-        <v>61302421121</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="8">
-        <v>61300821121</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>54</v>
+        <v>141</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="C21" s="5">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>58</v>
+        <v>142</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="C22" s="5">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>60</v>
+      <c r="E22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="8">
+        <v>61302421121</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="8">
+        <v>61300821121</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="1"/>
+      <c r="A24" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
+      <c r="E24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>63</v>
+        <v>145</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C25" s="5">
-        <v>0.5</v>
+        <v>16</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>67</v>
+        <v>13</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+        <v>146</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5">
+        <v>16</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E26" s="9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="9">
-        <v>11</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>75</v>
+      <c r="B28" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="E29" s="9" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="7"/>
+      <c r="E30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="9">
+        <v>11</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F35" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C37" s="5">
         <v>240</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C38" s="5">
         <v>300</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C39" s="5">
         <v>1</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F42" s="8">
         <v>451277</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="5">
-        <v>3090</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E43" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" s="5">
+        <v>3090</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1794,12 +1913,12 @@
       <c r="F44" s="1"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1807,24 +1926,45 @@
       <c r="F45" s="1"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="5"/>
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="5"/>
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1832,7 +1972,12 @@
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
+      <c r="A49" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1840,9 +1985,7 @@
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B50" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="B50" s="5"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1850,69 +1993,64 @@
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B51" s="5"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="B51" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="5"/>
+    <row r="52" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B52" s="18" t="s">
+        <v>192</v>
+      </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="2"/>
+      <c r="F52" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>122</v>
+      <c r="B53" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B54" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>121</v>
+      <c r="E54" s="1"/>
+      <c r="F54" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>123</v>
-      </c>
+      <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>124</v>
+      <c r="B56" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1921,6 +2059,7 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1936,27 +2075,54 @@
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="2"/>
+      <c r="E59" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="2"/>
+      <c r="E60" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -1971,7 +2137,7 @@
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="1"/>
+      <c r="B64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -1979,7 +2145,6 @@
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -1987,7 +2152,6 @@
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -1995,7 +2159,6 @@
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2003,9 +2166,6 @@
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2013,7 +2173,6 @@
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -2029,9 +2188,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -2039,9 +2196,7 @@
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2049,9 +2204,7 @@
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="5" t="s">
-        <v>127</v>
-      </c>
+      <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2059,8 +2212,8 @@
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="5" t="s">
-        <v>128</v>
+      <c r="B74" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2069,9 +2222,7 @@
       <c r="G74" s="2"/>
     </row>
     <row r="75" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B75" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -2087,7 +2238,9 @@
       <c r="G76" s="2"/>
     </row>
     <row r="77" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B77" s="1"/>
+      <c r="B77" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2095,7 +2248,9 @@
       <c r="G77" s="2"/>
     </row>
     <row r="78" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B78" s="1"/>
+      <c r="B78" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2103,7 +2258,9 @@
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="1"/>
+      <c r="B79" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -2111,7 +2268,9 @@
       <c r="G79" s="2"/>
     </row>
     <row r="80" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="1"/>
+      <c r="B80" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -2119,7 +2278,9 @@
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="1"/>
+      <c r="B81" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -9693,6 +9854,54 @@
       <c r="E1027" s="1"/>
       <c r="F1027" s="1"/>
       <c r="G1027" s="2"/>
+    </row>
+    <row r="1028" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+      <c r="E1028" s="1"/>
+      <c r="F1028" s="1"/>
+      <c r="G1028" s="2"/>
+    </row>
+    <row r="1029" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+      <c r="E1029" s="1"/>
+      <c r="F1029" s="1"/>
+      <c r="G1029" s="2"/>
+    </row>
+    <row r="1030" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+      <c r="E1030" s="1"/>
+      <c r="F1030" s="1"/>
+      <c r="G1030" s="2"/>
+    </row>
+    <row r="1031" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1"/>
+      <c r="F1031" s="1"/>
+      <c r="G1031" s="2"/>
+    </row>
+    <row r="1032" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+      <c r="E1032" s="1"/>
+      <c r="F1032" s="1"/>
+      <c r="G1032" s="2"/>
+    </row>
+    <row r="1033" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1033" s="1"/>
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+      <c r="E1033" s="1"/>
+      <c r="F1033" s="1"/>
+      <c r="G1033" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -9706,31 +9915,38 @@
     <hyperlink ref="G11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="G12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G20" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G36" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G37" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G39" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G53" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G54" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G21" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G22" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G23" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G25" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G35" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G36" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G38" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G41" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G42" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G43" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G46" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G60" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G14" r:id="rId34" xr:uid="{F819C3D6-85C8-457A-AF6C-4C156800226C}"/>
+    <hyperlink ref="G15" r:id="rId35" xr:uid="{6BF1E696-B3FB-46E5-B748-EB7EF30F6EAC}"/>
+    <hyperlink ref="G16" r:id="rId36" xr:uid="{D3678E6D-BD5A-4A25-A9D3-7BFD795BC701}"/>
+    <hyperlink ref="G17" r:id="rId37" xr:uid="{A9239624-81D8-4AC2-86CA-0FC2BEEA309D}"/>
+    <hyperlink ref="G52" r:id="rId38" xr:uid="{D58D8F0C-6926-4ED1-8708-F0795AAB528E}"/>
+    <hyperlink ref="G54" r:id="rId39" xr:uid="{D43E2B02-87E4-421A-88BB-2D199E95103B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>